<commit_message>
added titles row to excel
</commit_message>
<xml_diff>
--- a/xl_data/image17_0.xlsx
+++ b/xl_data/image17_0.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,55 +424,112 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Type of lecture</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Lecture Title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Resource Person Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Designation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>City,Country</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Course Code/Course Title</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Mode/Venue</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Coordinators</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>5th Module Panel Discussion</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>"Big Data Analytics"</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Shreya Mehta</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Cloud Architect</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Sydney, Australia</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>BCD9115 - Cybersecurity Fundamentals</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>9th March, 2024</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>2:00 PM to 4:00 PM</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>SJT401</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Dr. Preeti Singh, Dr. Karan Mehta, Dr. Puja Sharma and Dr. Mohan Kapoor</t>
         </is>

</xml_diff>